<commit_message>
[S2] MT: Modification des parametres pour les classes abstraites
</commit_message>
<xml_diff>
--- a/TimeTrackingSystem(TTS).xlsx
+++ b/TimeTrackingSystem(TTS).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\PolyDossier\H18\LOG2990\log2990-22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moncef\Documents\Poly\Hiver 2018\log2990\log2990-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -174,16 +174,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G36"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="#Sprint" dataDxfId="8"/>
-    <tableColumn id="2" name="Antoine" dataDxfId="7"/>
-    <tableColumn id="3" name="Samuel" dataDxfId="6"/>
-    <tableColumn id="4" name="Olivier" dataDxfId="5"/>
-    <tableColumn id="5" name="Monssaf" dataDxfId="4"/>
-    <tableColumn id="6" name="Claudia" dataDxfId="3"/>
-    <tableColumn id="7" name="William" dataDxfId="2"/>
+    <tableColumn id="1" name="#Sprint" dataDxfId="6"/>
+    <tableColumn id="2" name="Antoine" dataDxfId="5"/>
+    <tableColumn id="3" name="Samuel" dataDxfId="4"/>
+    <tableColumn id="4" name="Olivier" dataDxfId="3"/>
+    <tableColumn id="5" name="Monssaf" dataDxfId="2"/>
+    <tableColumn id="6" name="Claudia" dataDxfId="1"/>
+    <tableColumn id="7" name="William" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -489,15 +489,15 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -520,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -528,46 +528,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G3" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2">
-        <f>SUM(B2:B11)</f>
+        <f t="shared" ref="B12:G12" si="0">SUM(B2:B11)</f>
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f>SUM(C2:C11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <f>SUM(D2:D11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <f>SUM(E2:E11)</f>
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="2">
-        <f>SUM(F2:F11)</f>
-        <v>0</v>
-      </c>
       <c r="G12" s="2">
-        <f>SUM(G2:G11)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -576,12 +581,17 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -590,7 +600,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>